<commit_message>
separacion simulacion en funciones
</commit_message>
<xml_diff>
--- a/Tp3/Tabla de simulacion.xlsx
+++ b/Tp3/Tabla de simulacion.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="15">
   <si>
     <t>Iteracion</t>
   </si>
@@ -416,7 +416,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -573,9 +573,6 @@
       <c r="F4">
         <v>0.1461735928744393</v>
       </c>
-      <c r="G4" t="b">
-        <v>0</v>
-      </c>
       <c r="H4">
         <v>0.2542243735470147</v>
       </c>
@@ -734,9 +731,6 @@
       <c r="F8">
         <v>0.7992191914535041</v>
       </c>
-      <c r="G8" t="b">
-        <v>0</v>
-      </c>
       <c r="H8">
         <v>0.8661898433266887</v>
       </c>
@@ -772,9 +766,6 @@
       <c r="F9">
         <v>0.1143406707870935</v>
       </c>
-      <c r="G9" t="b">
-        <v>0</v>
-      </c>
       <c r="H9">
         <v>0.1958634574693732</v>
       </c>
@@ -874,6 +865,3382 @@
       </c>
       <c r="M11">
         <v>0.07142857142857142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>0.0903119738061291</v>
+      </c>
+      <c r="C12" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0.2278218019136226</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12">
+        <v>0.06738181922480679</v>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0.2526406424411292</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>200</v>
+      </c>
+      <c r="K12">
+        <v>400</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
+      </c>
+      <c r="M12">
+        <v>0.1333333333333333</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>0.8451740465079776</v>
+      </c>
+      <c r="C13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0.1699031914157111</v>
+      </c>
+      <c r="F13">
+        <v>0.0560959616301695</v>
+      </c>
+      <c r="H13">
+        <v>0.1822778657262263</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>400</v>
+      </c>
+      <c r="L13">
+        <v>2</v>
+      </c>
+      <c r="M13">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>0.9574865495802728</v>
+      </c>
+      <c r="C14" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0.587011829452687</v>
+      </c>
+      <c r="F14">
+        <v>0.7410928443720295</v>
+      </c>
+      <c r="H14">
+        <v>0.5256541555867068</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>400</v>
+      </c>
+      <c r="L14">
+        <v>2</v>
+      </c>
+      <c r="M14">
+        <v>0.1176470588235294</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>0.3559834839782393</v>
+      </c>
+      <c r="C15" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0.6606310318703495</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15">
+        <v>0.2959594607164776</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0.134107658955848</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>400</v>
+      </c>
+      <c r="L15">
+        <v>2</v>
+      </c>
+      <c r="M15">
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>0.3183839676095421</v>
+      </c>
+      <c r="C16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0.3391989663184694</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16">
+        <v>0.5562946502244391</v>
+      </c>
+      <c r="G16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0.610945089616083</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>400</v>
+      </c>
+      <c r="L16">
+        <v>2</v>
+      </c>
+      <c r="M16">
+        <v>0.1052631578947368</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>0.8946480434767501</v>
+      </c>
+      <c r="C17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0.2111625602698026</v>
+      </c>
+      <c r="F17">
+        <v>0.709017926258195</v>
+      </c>
+      <c r="H17">
+        <v>0.08868025733106821</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>400</v>
+      </c>
+      <c r="L17">
+        <v>2</v>
+      </c>
+      <c r="M17">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>0.9274511817091716</v>
+      </c>
+      <c r="C18" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0.03907280950137082</v>
+      </c>
+      <c r="F18">
+        <v>0.1671148600517429</v>
+      </c>
+      <c r="H18">
+        <v>0.2772559699070153</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>400</v>
+      </c>
+      <c r="L18">
+        <v>2</v>
+      </c>
+      <c r="M18">
+        <v>0.09523809523809523</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>0.6365528489020295</v>
+      </c>
+      <c r="C19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>0.5966725951186698</v>
+      </c>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19">
+        <v>0.7680727534361818</v>
+      </c>
+      <c r="G19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0.3974196050989756</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>400</v>
+      </c>
+      <c r="L19">
+        <v>2</v>
+      </c>
+      <c r="M19">
+        <v>0.09090909090909091</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>0.4420978247008245</v>
+      </c>
+      <c r="C20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>0.07127817611095821</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20">
+        <v>0.8903869991928866</v>
+      </c>
+      <c r="G20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0.7174323958999965</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>400</v>
+      </c>
+      <c r="L20">
+        <v>2</v>
+      </c>
+      <c r="M20">
+        <v>0.08695652173913043</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21">
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <v>0.7740383119266477</v>
+      </c>
+      <c r="C21" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0.2359400812744188</v>
+      </c>
+      <c r="F21">
+        <v>0.1216303611571934</v>
+      </c>
+      <c r="H21">
+        <v>0.4059378383584892</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>400</v>
+      </c>
+      <c r="L21">
+        <v>2</v>
+      </c>
+      <c r="M21">
+        <v>0.08333333333333333</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22">
+        <v>25</v>
+      </c>
+      <c r="B22">
+        <v>0.5446755600629632</v>
+      </c>
+      <c r="C22" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0.9836090967507382</v>
+      </c>
+      <c r="E22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22">
+        <v>0.5916918049914037</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0.7941624836424515</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>400</v>
+      </c>
+      <c r="L22">
+        <v>2</v>
+      </c>
+      <c r="M22">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <v>0.1070740653392621</v>
+      </c>
+      <c r="C23" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0.3192221286969236</v>
+      </c>
+      <c r="E23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23">
+        <v>0.515913834739491</v>
+      </c>
+      <c r="G23" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0.8449477035977715</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>400</v>
+      </c>
+      <c r="L23">
+        <v>2</v>
+      </c>
+      <c r="M23">
+        <v>0.07692307692307693</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24">
+        <v>27</v>
+      </c>
+      <c r="B24">
+        <v>0.3954193722932251</v>
+      </c>
+      <c r="C24" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>0.2022494624418835</v>
+      </c>
+      <c r="E24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24">
+        <v>0.08632843331531215</v>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>0.2145044911323493</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>200</v>
+      </c>
+      <c r="K24">
+        <v>600</v>
+      </c>
+      <c r="L24">
+        <v>3</v>
+      </c>
+      <c r="M24">
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25">
+        <v>28</v>
+      </c>
+      <c r="B25">
+        <v>0.1882111245368662</v>
+      </c>
+      <c r="C25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>0.8706017731461435</v>
+      </c>
+      <c r="E25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25">
+        <v>0.8445718688330693</v>
+      </c>
+      <c r="G25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0.2336840159979071</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>600</v>
+      </c>
+      <c r="L25">
+        <v>3</v>
+      </c>
+      <c r="M25">
+        <v>0.1071428571428571</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26">
+        <v>29</v>
+      </c>
+      <c r="B26">
+        <v>0.5404405796921191</v>
+      </c>
+      <c r="C26" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>0.6263259871233494</v>
+      </c>
+      <c r="E26" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26">
+        <v>0.1112382226081174</v>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>0.7656792064431199</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+      <c r="J26">
+        <v>400</v>
+      </c>
+      <c r="K26">
+        <v>1000</v>
+      </c>
+      <c r="L26">
+        <v>4</v>
+      </c>
+      <c r="M26">
+        <v>0.1379310344827586</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27">
+        <v>30</v>
+      </c>
+      <c r="B27">
+        <v>0.2392767817731829</v>
+      </c>
+      <c r="C27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>0.900286406729785</v>
+      </c>
+      <c r="E27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27">
+        <v>0.5363230008458487</v>
+      </c>
+      <c r="G27" t="b">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0.3079873151910195</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>1000</v>
+      </c>
+      <c r="L27">
+        <v>4</v>
+      </c>
+      <c r="M27">
+        <v>0.1333333333333333</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28">
+        <v>31</v>
+      </c>
+      <c r="B28">
+        <v>0.960792649991501</v>
+      </c>
+      <c r="C28" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0.3874893612285695</v>
+      </c>
+      <c r="F28">
+        <v>0.03471519726390293</v>
+      </c>
+      <c r="H28">
+        <v>0.6775841561824575</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>1000</v>
+      </c>
+      <c r="L28">
+        <v>4</v>
+      </c>
+      <c r="M28">
+        <v>0.1290322580645161</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29">
+        <v>32</v>
+      </c>
+      <c r="B29">
+        <v>0.7135211051905317</v>
+      </c>
+      <c r="C29" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0.1344474597287927</v>
+      </c>
+      <c r="F29">
+        <v>0.6998907813392948</v>
+      </c>
+      <c r="H29">
+        <v>0.2525143526262679</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>1000</v>
+      </c>
+      <c r="L29">
+        <v>4</v>
+      </c>
+      <c r="M29">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30">
+        <v>33</v>
+      </c>
+      <c r="B30">
+        <v>0.1526822250907959</v>
+      </c>
+      <c r="C30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>0.1440045225188422</v>
+      </c>
+      <c r="E30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30">
+        <v>0.9006822396608452</v>
+      </c>
+      <c r="G30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0.7888946405283235</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>1000</v>
+      </c>
+      <c r="L30">
+        <v>4</v>
+      </c>
+      <c r="M30">
+        <v>0.1212121212121212</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31">
+        <v>34</v>
+      </c>
+      <c r="B31">
+        <v>0.9016895655051014</v>
+      </c>
+      <c r="C31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0.5977547694969387</v>
+      </c>
+      <c r="F31">
+        <v>0.3180015005719278</v>
+      </c>
+      <c r="H31">
+        <v>0.6208150657105606</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>1000</v>
+      </c>
+      <c r="L31">
+        <v>4</v>
+      </c>
+      <c r="M31">
+        <v>0.1176470588235294</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32">
+        <v>35</v>
+      </c>
+      <c r="B32">
+        <v>0.02639409173509111</v>
+      </c>
+      <c r="C32" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>0.3080427899393573</v>
+      </c>
+      <c r="E32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32">
+        <v>0.8043325896630625</v>
+      </c>
+      <c r="G32" t="b">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0.9898251951669944</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>1000</v>
+      </c>
+      <c r="L32">
+        <v>4</v>
+      </c>
+      <c r="M32">
+        <v>0.1142857142857143</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33">
+        <v>36</v>
+      </c>
+      <c r="B33">
+        <v>0.006464173298180498</v>
+      </c>
+      <c r="C33" t="b">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>0.306984754839873</v>
+      </c>
+      <c r="E33" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33">
+        <v>0.312432772418891</v>
+      </c>
+      <c r="G33" t="b">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0.6446658169435185</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>1000</v>
+      </c>
+      <c r="L33">
+        <v>4</v>
+      </c>
+      <c r="M33">
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34">
+        <v>37</v>
+      </c>
+      <c r="B34">
+        <v>0.3962769453001561</v>
+      </c>
+      <c r="C34" t="b">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>0.6366508777376779</v>
+      </c>
+      <c r="E34" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34">
+        <v>0.7013718805567628</v>
+      </c>
+      <c r="G34" t="b">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0.9758175706532025</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>1000</v>
+      </c>
+      <c r="L34">
+        <v>4</v>
+      </c>
+      <c r="M34">
+        <v>0.1081081081081081</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35">
+        <v>38</v>
+      </c>
+      <c r="B35">
+        <v>0.9126337409358529</v>
+      </c>
+      <c r="C35" t="b">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0.4523861090278375</v>
+      </c>
+      <c r="F35">
+        <v>0.1580084164322526</v>
+      </c>
+      <c r="H35">
+        <v>0.302733769827954</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>1000</v>
+      </c>
+      <c r="L35">
+        <v>4</v>
+      </c>
+      <c r="M35">
+        <v>0.1052631578947368</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36">
+        <v>39</v>
+      </c>
+      <c r="B36">
+        <v>0.8240025114309678</v>
+      </c>
+      <c r="C36" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0.5896628402009718</v>
+      </c>
+      <c r="F36">
+        <v>0.3966106250777754</v>
+      </c>
+      <c r="H36">
+        <v>0.03382373389551074</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>1000</v>
+      </c>
+      <c r="L36">
+        <v>4</v>
+      </c>
+      <c r="M36">
+        <v>0.1025641025641026</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37">
+        <v>40</v>
+      </c>
+      <c r="B37">
+        <v>0.2026721460112825</v>
+      </c>
+      <c r="C37" t="b">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>0.4207602513223907</v>
+      </c>
+      <c r="E37" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37">
+        <v>0.4212821620200965</v>
+      </c>
+      <c r="G37" t="b">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0.1258892902075899</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>1000</v>
+      </c>
+      <c r="L37">
+        <v>4</v>
+      </c>
+      <c r="M37">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38">
+        <v>41</v>
+      </c>
+      <c r="B38">
+        <v>0.3541760709111063</v>
+      </c>
+      <c r="C38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>0.1523895000109626</v>
+      </c>
+      <c r="E38" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38">
+        <v>0.7821498418284316</v>
+      </c>
+      <c r="G38" t="b">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0.2298356332266576</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>1000</v>
+      </c>
+      <c r="L38">
+        <v>4</v>
+      </c>
+      <c r="M38">
+        <v>0.0975609756097561</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39">
+        <v>42</v>
+      </c>
+      <c r="B39">
+        <v>0.1424255928274804</v>
+      </c>
+      <c r="C39" t="b">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>0.3772734118561697</v>
+      </c>
+      <c r="E39" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39">
+        <v>0.546584986156887</v>
+      </c>
+      <c r="G39" t="b">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0.06461652680574337</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>1000</v>
+      </c>
+      <c r="L39">
+        <v>4</v>
+      </c>
+      <c r="M39">
+        <v>0.09523809523809523</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40">
+        <v>43</v>
+      </c>
+      <c r="B40">
+        <v>0.7389838265466889</v>
+      </c>
+      <c r="C40" t="b">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0.9599744450604392</v>
+      </c>
+      <c r="F40">
+        <v>0.2524336054206205</v>
+      </c>
+      <c r="H40">
+        <v>0.1638572119072806</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>1000</v>
+      </c>
+      <c r="L40">
+        <v>4</v>
+      </c>
+      <c r="M40">
+        <v>0.09302325581395349</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41">
+        <v>44</v>
+      </c>
+      <c r="B41">
+        <v>0.3593626325039112</v>
+      </c>
+      <c r="C41" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>0.1806869843963294</v>
+      </c>
+      <c r="E41" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41">
+        <v>0.5330577892779462</v>
+      </c>
+      <c r="G41" t="b">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0.9444539695583009</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>1000</v>
+      </c>
+      <c r="L41">
+        <v>4</v>
+      </c>
+      <c r="M41">
+        <v>0.09090909090909091</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42">
+        <v>45</v>
+      </c>
+      <c r="B42">
+        <v>0.6956458622673749</v>
+      </c>
+      <c r="C42" t="b">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>0.333426899248279</v>
+      </c>
+      <c r="E42" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42">
+        <v>0.5617543785966028</v>
+      </c>
+      <c r="G42" t="b">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0.1751984194428522</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>1000</v>
+      </c>
+      <c r="L42">
+        <v>4</v>
+      </c>
+      <c r="M42">
+        <v>0.08888888888888889</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43">
+        <v>46</v>
+      </c>
+      <c r="B43">
+        <v>0.1628099076792077</v>
+      </c>
+      <c r="C43" t="b">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>0.7898365708545169</v>
+      </c>
+      <c r="E43" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43">
+        <v>0.5911322510179983</v>
+      </c>
+      <c r="G43" t="b">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0.4610733633886714</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>1000</v>
+      </c>
+      <c r="L43">
+        <v>4</v>
+      </c>
+      <c r="M43">
+        <v>0.08695652173913043</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44">
+        <v>47</v>
+      </c>
+      <c r="B44">
+        <v>0.1903547252167433</v>
+      </c>
+      <c r="C44" t="b">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>0.9243888724625018</v>
+      </c>
+      <c r="E44" t="s">
+        <v>14</v>
+      </c>
+      <c r="F44">
+        <v>0.1028399446212397</v>
+      </c>
+      <c r="G44" t="b">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>0.537677060367592</v>
+      </c>
+      <c r="I44">
+        <v>3</v>
+      </c>
+      <c r="J44">
+        <v>600</v>
+      </c>
+      <c r="K44">
+        <v>1600</v>
+      </c>
+      <c r="L44">
+        <v>5</v>
+      </c>
+      <c r="M44">
+        <v>0.1063829787234043</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45">
+        <v>48</v>
+      </c>
+      <c r="B45">
+        <v>0.4002734095978788</v>
+      </c>
+      <c r="C45" t="b">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>0.6772241532499909</v>
+      </c>
+      <c r="E45" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45">
+        <v>0.6976975431357597</v>
+      </c>
+      <c r="G45" t="b">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0.2374113042062048</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>1600</v>
+      </c>
+      <c r="L45">
+        <v>5</v>
+      </c>
+      <c r="M45">
+        <v>0.1041666666666667</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46">
+        <v>49</v>
+      </c>
+      <c r="B46">
+        <v>0.3899941088865178</v>
+      </c>
+      <c r="C46" t="b">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>0.8936859815855724</v>
+      </c>
+      <c r="E46" t="s">
+        <v>14</v>
+      </c>
+      <c r="F46">
+        <v>0.6360210689025552</v>
+      </c>
+      <c r="G46" t="b">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0.3887978957568531</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>1600</v>
+      </c>
+      <c r="L46">
+        <v>5</v>
+      </c>
+      <c r="M46">
+        <v>0.1020408163265306</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47">
+        <v>50</v>
+      </c>
+      <c r="B47">
+        <v>0.4601351291045154</v>
+      </c>
+      <c r="C47" t="b">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>0.6459548018571334</v>
+      </c>
+      <c r="E47" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47">
+        <v>0.06927223312108899</v>
+      </c>
+      <c r="G47" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <v>0.5212703794447788</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+      <c r="J47">
+        <v>200</v>
+      </c>
+      <c r="K47">
+        <v>1800</v>
+      </c>
+      <c r="L47">
+        <v>6</v>
+      </c>
+      <c r="M47">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48">
+        <v>51</v>
+      </c>
+      <c r="B48">
+        <v>0.5892522179862945</v>
+      </c>
+      <c r="C48" t="b">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>0.8631297303679617</v>
+      </c>
+      <c r="E48" t="s">
+        <v>14</v>
+      </c>
+      <c r="F48">
+        <v>0.1307746035060877</v>
+      </c>
+      <c r="G48" t="b">
+        <v>1</v>
+      </c>
+      <c r="H48">
+        <v>0.3752954482184863</v>
+      </c>
+      <c r="I48">
+        <v>2</v>
+      </c>
+      <c r="J48">
+        <v>400</v>
+      </c>
+      <c r="K48">
+        <v>2200</v>
+      </c>
+      <c r="L48">
+        <v>7</v>
+      </c>
+      <c r="M48">
+        <v>0.1372549019607843</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49">
+        <v>52</v>
+      </c>
+      <c r="B49">
+        <v>0.5479631720746255</v>
+      </c>
+      <c r="C49" t="b">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>0.2026367073277549</v>
+      </c>
+      <c r="E49" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49">
+        <v>0.691951343786576</v>
+      </c>
+      <c r="G49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0.2066489458519248</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>2200</v>
+      </c>
+      <c r="L49">
+        <v>7</v>
+      </c>
+      <c r="M49">
+        <v>0.1346153846153846</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50">
+        <v>53</v>
+      </c>
+      <c r="B50">
+        <v>0.119707454779331</v>
+      </c>
+      <c r="C50" t="b">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>0.3831439742260313</v>
+      </c>
+      <c r="E50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F50">
+        <v>0.1008367809747589</v>
+      </c>
+      <c r="G50" t="b">
+        <v>1</v>
+      </c>
+      <c r="H50">
+        <v>0.3249127803300795</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+      <c r="J50">
+        <v>200</v>
+      </c>
+      <c r="K50">
+        <v>2400</v>
+      </c>
+      <c r="L50">
+        <v>8</v>
+      </c>
+      <c r="M50">
+        <v>0.1509433962264151</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51">
+        <v>54</v>
+      </c>
+      <c r="B51">
+        <v>0.696494083627865</v>
+      </c>
+      <c r="C51" t="b">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>0.841446129116328</v>
+      </c>
+      <c r="E51" t="s">
+        <v>14</v>
+      </c>
+      <c r="F51">
+        <v>0.3247780858825783</v>
+      </c>
+      <c r="G51" t="b">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>0.7808194469523784</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <v>2400</v>
+      </c>
+      <c r="L51">
+        <v>8</v>
+      </c>
+      <c r="M51">
+        <v>0.1481481481481481</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52">
+        <v>55</v>
+      </c>
+      <c r="B52">
+        <v>0.08224035407169661</v>
+      </c>
+      <c r="C52" t="b">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>0.4349751924344573</v>
+      </c>
+      <c r="E52" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52">
+        <v>0.8212453248943509</v>
+      </c>
+      <c r="G52" t="b">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>0.5209885887104938</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52">
+        <v>2400</v>
+      </c>
+      <c r="L52">
+        <v>8</v>
+      </c>
+      <c r="M52">
+        <v>0.1454545454545454</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53">
+        <v>56</v>
+      </c>
+      <c r="B53">
+        <v>0.8781612926574694</v>
+      </c>
+      <c r="C53" t="b">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0.6821724686994568</v>
+      </c>
+      <c r="F53">
+        <v>0.8448964117542926</v>
+      </c>
+      <c r="H53">
+        <v>0.6265084226517427</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53">
+        <v>2400</v>
+      </c>
+      <c r="L53">
+        <v>8</v>
+      </c>
+      <c r="M53">
+        <v>0.1428571428571428</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54">
+        <v>57</v>
+      </c>
+      <c r="B54">
+        <v>0.1741995226612307</v>
+      </c>
+      <c r="C54" t="b">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>0.7965314957631952</v>
+      </c>
+      <c r="E54" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54">
+        <v>0.9744836378581767</v>
+      </c>
+      <c r="G54" t="b">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0.8092660313324909</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>2400</v>
+      </c>
+      <c r="L54">
+        <v>8</v>
+      </c>
+      <c r="M54">
+        <v>0.1403508771929824</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55">
+        <v>58</v>
+      </c>
+      <c r="B55">
+        <v>0.2066459993848122</v>
+      </c>
+      <c r="C55" t="b">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>0.6691341138722559</v>
+      </c>
+      <c r="E55" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55">
+        <v>0.752441792547117</v>
+      </c>
+      <c r="G55" t="b">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>0.5611808754111618</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>2400</v>
+      </c>
+      <c r="L55">
+        <v>8</v>
+      </c>
+      <c r="M55">
+        <v>0.1379310344827586</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
+      <c r="A56">
+        <v>59</v>
+      </c>
+      <c r="B56">
+        <v>0.3621882693060748</v>
+      </c>
+      <c r="C56" t="b">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>0.3905741430739561</v>
+      </c>
+      <c r="E56" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56">
+        <v>0.4421866339112439</v>
+      </c>
+      <c r="G56" t="b">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>0.6838266195293725</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <v>2400</v>
+      </c>
+      <c r="L56">
+        <v>8</v>
+      </c>
+      <c r="M56">
+        <v>0.1355932203389831</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
+      <c r="A57">
+        <v>60</v>
+      </c>
+      <c r="B57">
+        <v>0.4255467730746658</v>
+      </c>
+      <c r="C57" t="b">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>0.9207650809457619</v>
+      </c>
+      <c r="E57" t="s">
+        <v>14</v>
+      </c>
+      <c r="F57">
+        <v>0.7321051158566984</v>
+      </c>
+      <c r="G57" t="b">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>0.822562409606987</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <v>2400</v>
+      </c>
+      <c r="L57">
+        <v>8</v>
+      </c>
+      <c r="M57">
+        <v>0.1333333333333333</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
+      <c r="A58">
+        <v>61</v>
+      </c>
+      <c r="B58">
+        <v>0.04056496941522048</v>
+      </c>
+      <c r="C58" t="b">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>0.5752866972360814</v>
+      </c>
+      <c r="E58" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58">
+        <v>0.2420429657845243</v>
+      </c>
+      <c r="G58" t="b">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>0.3126378778758384</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+      <c r="K58">
+        <v>2400</v>
+      </c>
+      <c r="L58">
+        <v>8</v>
+      </c>
+      <c r="M58">
+        <v>0.1311475409836066</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
+      <c r="A59">
+        <v>62</v>
+      </c>
+      <c r="B59">
+        <v>0.8251801405145306</v>
+      </c>
+      <c r="C59" t="b">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0.06628160367546476</v>
+      </c>
+      <c r="F59">
+        <v>0.643123040444571</v>
+      </c>
+      <c r="H59">
+        <v>0.110429190192358</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <v>2400</v>
+      </c>
+      <c r="L59">
+        <v>8</v>
+      </c>
+      <c r="M59">
+        <v>0.1290322580645161</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
+      <c r="A60">
+        <v>63</v>
+      </c>
+      <c r="B60">
+        <v>0.07410232406308181</v>
+      </c>
+      <c r="C60" t="b">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>0.6465599012247776</v>
+      </c>
+      <c r="E60" t="s">
+        <v>13</v>
+      </c>
+      <c r="F60">
+        <v>0.6470210845565256</v>
+      </c>
+      <c r="G60" t="b">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>0.6433313604169107</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <v>2400</v>
+      </c>
+      <c r="L60">
+        <v>8</v>
+      </c>
+      <c r="M60">
+        <v>0.126984126984127</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
+      <c r="A61">
+        <v>64</v>
+      </c>
+      <c r="B61">
+        <v>0.8560590344430996</v>
+      </c>
+      <c r="C61" t="b">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0.1633826854661218</v>
+      </c>
+      <c r="F61">
+        <v>0.2800594655216415</v>
+      </c>
+      <c r="H61">
+        <v>0.4369205558522329</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+      <c r="K61">
+        <v>2400</v>
+      </c>
+      <c r="L61">
+        <v>8</v>
+      </c>
+      <c r="M61">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13">
+      <c r="A62">
+        <v>65</v>
+      </c>
+      <c r="B62">
+        <v>0.6473657561943105</v>
+      </c>
+      <c r="C62" t="b">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>0.9580190796195163</v>
+      </c>
+      <c r="E62" t="s">
+        <v>14</v>
+      </c>
+      <c r="F62">
+        <v>0.535473635158551</v>
+      </c>
+      <c r="G62" t="b">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>0.8710694373003678</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+      <c r="K62">
+        <v>2400</v>
+      </c>
+      <c r="L62">
+        <v>8</v>
+      </c>
+      <c r="M62">
+        <v>0.1230769230769231</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13">
+      <c r="A63">
+        <v>66</v>
+      </c>
+      <c r="B63">
+        <v>0.006377464689079737</v>
+      </c>
+      <c r="C63" t="b">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>0.2265962825809129</v>
+      </c>
+      <c r="E63" t="s">
+        <v>13</v>
+      </c>
+      <c r="F63">
+        <v>0.3201662019055165</v>
+      </c>
+      <c r="G63" t="b">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>0.890907164386014</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>0</v>
+      </c>
+      <c r="K63">
+        <v>2400</v>
+      </c>
+      <c r="L63">
+        <v>8</v>
+      </c>
+      <c r="M63">
+        <v>0.1212121212121212</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13">
+      <c r="A64">
+        <v>67</v>
+      </c>
+      <c r="B64">
+        <v>0.09206180347263215</v>
+      </c>
+      <c r="C64" t="b">
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>0.9050149757187455</v>
+      </c>
+      <c r="E64" t="s">
+        <v>14</v>
+      </c>
+      <c r="F64">
+        <v>0.103302744484626</v>
+      </c>
+      <c r="G64" t="b">
+        <v>1</v>
+      </c>
+      <c r="H64">
+        <v>0.1176253073197642</v>
+      </c>
+      <c r="I64">
+        <v>2</v>
+      </c>
+      <c r="J64">
+        <v>400</v>
+      </c>
+      <c r="K64">
+        <v>2800</v>
+      </c>
+      <c r="L64">
+        <v>9</v>
+      </c>
+      <c r="M64">
+        <v>0.1343283582089552</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13">
+      <c r="A65">
+        <v>68</v>
+      </c>
+      <c r="B65">
+        <v>0.9930510364153214</v>
+      </c>
+      <c r="C65" t="b">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0.4758440301210837</v>
+      </c>
+      <c r="F65">
+        <v>0.7453936669337666</v>
+      </c>
+      <c r="H65">
+        <v>0.1708892700323977</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+      <c r="K65">
+        <v>2800</v>
+      </c>
+      <c r="L65">
+        <v>9</v>
+      </c>
+      <c r="M65">
+        <v>0.1323529411764706</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13">
+      <c r="A66">
+        <v>69</v>
+      </c>
+      <c r="B66">
+        <v>0.9390636680884263</v>
+      </c>
+      <c r="C66" t="b">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0.6378232357498121</v>
+      </c>
+      <c r="F66">
+        <v>0.2957750451774269</v>
+      </c>
+      <c r="H66">
+        <v>0.8609838079261106</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
+      <c r="K66">
+        <v>2800</v>
+      </c>
+      <c r="L66">
+        <v>9</v>
+      </c>
+      <c r="M66">
+        <v>0.1304347826086956</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13">
+      <c r="A67">
+        <v>70</v>
+      </c>
+      <c r="B67">
+        <v>0.9916131581210105</v>
+      </c>
+      <c r="C67" t="b">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0.0319627247445432</v>
+      </c>
+      <c r="F67">
+        <v>0.9946499279032326</v>
+      </c>
+      <c r="H67">
+        <v>0.3792974557147272</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+      <c r="K67">
+        <v>2800</v>
+      </c>
+      <c r="L67">
+        <v>9</v>
+      </c>
+      <c r="M67">
+        <v>0.1285714285714286</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13">
+      <c r="A68">
+        <v>71</v>
+      </c>
+      <c r="B68">
+        <v>0.3067758379703885</v>
+      </c>
+      <c r="C68" t="b">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <v>0.5461796641960343</v>
+      </c>
+      <c r="E68" t="s">
+        <v>13</v>
+      </c>
+      <c r="F68">
+        <v>0.751922883412969</v>
+      </c>
+      <c r="G68" t="b">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>0.2973072226801475</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+      <c r="J68">
+        <v>0</v>
+      </c>
+      <c r="K68">
+        <v>2800</v>
+      </c>
+      <c r="L68">
+        <v>9</v>
+      </c>
+      <c r="M68">
+        <v>0.1267605633802817</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13">
+      <c r="A69">
+        <v>72</v>
+      </c>
+      <c r="B69">
+        <v>0.7490546938475547</v>
+      </c>
+      <c r="C69" t="b">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0.791721164055208</v>
+      </c>
+      <c r="F69">
+        <v>0.8487659567866885</v>
+      </c>
+      <c r="H69">
+        <v>0.8883166146013394</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+      <c r="J69">
+        <v>0</v>
+      </c>
+      <c r="K69">
+        <v>2800</v>
+      </c>
+      <c r="L69">
+        <v>9</v>
+      </c>
+      <c r="M69">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13">
+      <c r="A70">
+        <v>73</v>
+      </c>
+      <c r="B70">
+        <v>0.5590740123285851</v>
+      </c>
+      <c r="C70" t="b">
+        <v>1</v>
+      </c>
+      <c r="D70">
+        <v>0.5267358292364898</v>
+      </c>
+      <c r="E70" t="s">
+        <v>13</v>
+      </c>
+      <c r="F70">
+        <v>0.1891590801295043</v>
+      </c>
+      <c r="G70" t="b">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>0.3819508490001673</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70">
+        <v>0</v>
+      </c>
+      <c r="K70">
+        <v>2800</v>
+      </c>
+      <c r="L70">
+        <v>9</v>
+      </c>
+      <c r="M70">
+        <v>0.1232876712328767</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13">
+      <c r="A71">
+        <v>74</v>
+      </c>
+      <c r="B71">
+        <v>0.3963431291886252</v>
+      </c>
+      <c r="C71" t="b">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>0.3090090024830011</v>
+      </c>
+      <c r="E71" t="s">
+        <v>13</v>
+      </c>
+      <c r="F71">
+        <v>0.6188187202769483</v>
+      </c>
+      <c r="G71" t="b">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>0.5944415849986184</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+      <c r="K71">
+        <v>2800</v>
+      </c>
+      <c r="L71">
+        <v>9</v>
+      </c>
+      <c r="M71">
+        <v>0.1216216216216216</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13">
+      <c r="A72">
+        <v>75</v>
+      </c>
+      <c r="B72">
+        <v>0.6998409146715343</v>
+      </c>
+      <c r="C72" t="b">
+        <v>1</v>
+      </c>
+      <c r="D72">
+        <v>0.9051571297331431</v>
+      </c>
+      <c r="E72" t="s">
+        <v>14</v>
+      </c>
+      <c r="F72">
+        <v>0.6175381050090423</v>
+      </c>
+      <c r="G72" t="b">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>0.01035966898458995</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+      <c r="K72">
+        <v>2800</v>
+      </c>
+      <c r="L72">
+        <v>9</v>
+      </c>
+      <c r="M72">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13">
+      <c r="A73">
+        <v>76</v>
+      </c>
+      <c r="B73">
+        <v>0.07449847105758012</v>
+      </c>
+      <c r="C73" t="b">
+        <v>1</v>
+      </c>
+      <c r="D73">
+        <v>0.6749685546185691</v>
+      </c>
+      <c r="E73" t="s">
+        <v>13</v>
+      </c>
+      <c r="F73">
+        <v>0.3800755424142278</v>
+      </c>
+      <c r="G73" t="b">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>0.7038497727951589</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+      <c r="K73">
+        <v>2800</v>
+      </c>
+      <c r="L73">
+        <v>9</v>
+      </c>
+      <c r="M73">
+        <v>0.1184210526315789</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13">
+      <c r="A74">
+        <v>77</v>
+      </c>
+      <c r="B74">
+        <v>0.2483324506924771</v>
+      </c>
+      <c r="C74" t="b">
+        <v>1</v>
+      </c>
+      <c r="D74">
+        <v>0.8252280572765064</v>
+      </c>
+      <c r="E74" t="s">
+        <v>14</v>
+      </c>
+      <c r="F74">
+        <v>0.1118857225002086</v>
+      </c>
+      <c r="G74" t="b">
+        <v>1</v>
+      </c>
+      <c r="H74">
+        <v>0.03136747947669616</v>
+      </c>
+      <c r="I74">
+        <v>1</v>
+      </c>
+      <c r="J74">
+        <v>200</v>
+      </c>
+      <c r="K74">
+        <v>3000</v>
+      </c>
+      <c r="L74">
+        <v>10</v>
+      </c>
+      <c r="M74">
+        <v>0.1298701298701299</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13">
+      <c r="A75">
+        <v>78</v>
+      </c>
+      <c r="B75">
+        <v>0.9119996840757302</v>
+      </c>
+      <c r="C75" t="b">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0.1974703609982668</v>
+      </c>
+      <c r="F75">
+        <v>0.6533097016641062</v>
+      </c>
+      <c r="H75">
+        <v>0.999309519548751</v>
+      </c>
+      <c r="I75">
+        <v>0</v>
+      </c>
+      <c r="J75">
+        <v>0</v>
+      </c>
+      <c r="K75">
+        <v>3000</v>
+      </c>
+      <c r="L75">
+        <v>10</v>
+      </c>
+      <c r="M75">
+        <v>0.1282051282051282</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13">
+      <c r="A76">
+        <v>79</v>
+      </c>
+      <c r="B76">
+        <v>0.3286708834903335</v>
+      </c>
+      <c r="C76" t="b">
+        <v>1</v>
+      </c>
+      <c r="D76">
+        <v>0.3818401410650285</v>
+      </c>
+      <c r="E76" t="s">
+        <v>13</v>
+      </c>
+      <c r="F76">
+        <v>0.3813152123339726</v>
+      </c>
+      <c r="G76" t="b">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>0.4224876679323003</v>
+      </c>
+      <c r="I76">
+        <v>0</v>
+      </c>
+      <c r="J76">
+        <v>0</v>
+      </c>
+      <c r="K76">
+        <v>3000</v>
+      </c>
+      <c r="L76">
+        <v>10</v>
+      </c>
+      <c r="M76">
+        <v>0.1265822784810127</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13">
+      <c r="A77">
+        <v>80</v>
+      </c>
+      <c r="B77">
+        <v>0.4012819523158934</v>
+      </c>
+      <c r="C77" t="b">
+        <v>1</v>
+      </c>
+      <c r="D77">
+        <v>0.4225892100967206</v>
+      </c>
+      <c r="E77" t="s">
+        <v>13</v>
+      </c>
+      <c r="F77">
+        <v>0.7824573908137478</v>
+      </c>
+      <c r="G77" t="b">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <v>0.4201617714108209</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+      <c r="J77">
+        <v>0</v>
+      </c>
+      <c r="K77">
+        <v>3000</v>
+      </c>
+      <c r="L77">
+        <v>10</v>
+      </c>
+      <c r="M77">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13">
+      <c r="A78">
+        <v>81</v>
+      </c>
+      <c r="B78">
+        <v>0.6587277458419154</v>
+      </c>
+      <c r="C78" t="b">
+        <v>1</v>
+      </c>
+      <c r="D78">
+        <v>0.7085435299827092</v>
+      </c>
+      <c r="E78" t="s">
+        <v>13</v>
+      </c>
+      <c r="F78">
+        <v>0.5435325093036855</v>
+      </c>
+      <c r="G78" t="b">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>0.8373544058911517</v>
+      </c>
+      <c r="I78">
+        <v>0</v>
+      </c>
+      <c r="J78">
+        <v>0</v>
+      </c>
+      <c r="K78">
+        <v>3000</v>
+      </c>
+      <c r="L78">
+        <v>10</v>
+      </c>
+      <c r="M78">
+        <v>0.1234567901234568</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13">
+      <c r="A79">
+        <v>82</v>
+      </c>
+      <c r="B79">
+        <v>0.25147485632286</v>
+      </c>
+      <c r="C79" t="b">
+        <v>1</v>
+      </c>
+      <c r="D79">
+        <v>0.5143647554285893</v>
+      </c>
+      <c r="E79" t="s">
+        <v>13</v>
+      </c>
+      <c r="F79">
+        <v>0.3710033804881114</v>
+      </c>
+      <c r="G79" t="b">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>0.7636796719524486</v>
+      </c>
+      <c r="I79">
+        <v>0</v>
+      </c>
+      <c r="J79">
+        <v>0</v>
+      </c>
+      <c r="K79">
+        <v>3000</v>
+      </c>
+      <c r="L79">
+        <v>10</v>
+      </c>
+      <c r="M79">
+        <v>0.1219512195121951</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13">
+      <c r="A80">
+        <v>83</v>
+      </c>
+      <c r="B80">
+        <v>0.83959977103431</v>
+      </c>
+      <c r="C80" t="b">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0.8043396228770571</v>
+      </c>
+      <c r="F80">
+        <v>0.6466084108362197</v>
+      </c>
+      <c r="H80">
+        <v>0.9275054556345484</v>
+      </c>
+      <c r="I80">
+        <v>0</v>
+      </c>
+      <c r="J80">
+        <v>0</v>
+      </c>
+      <c r="K80">
+        <v>3000</v>
+      </c>
+      <c r="L80">
+        <v>10</v>
+      </c>
+      <c r="M80">
+        <v>0.1204819277108434</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13">
+      <c r="A81">
+        <v>84</v>
+      </c>
+      <c r="B81">
+        <v>0.2278749274134539</v>
+      </c>
+      <c r="C81" t="b">
+        <v>1</v>
+      </c>
+      <c r="D81">
+        <v>0.07704385049116602</v>
+      </c>
+      <c r="E81" t="s">
+        <v>13</v>
+      </c>
+      <c r="F81">
+        <v>0.6796058251107534</v>
+      </c>
+      <c r="G81" t="b">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>0.9949279800078658</v>
+      </c>
+      <c r="I81">
+        <v>0</v>
+      </c>
+      <c r="J81">
+        <v>0</v>
+      </c>
+      <c r="K81">
+        <v>3000</v>
+      </c>
+      <c r="L81">
+        <v>10</v>
+      </c>
+      <c r="M81">
+        <v>0.119047619047619</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13">
+      <c r="A82">
+        <v>85</v>
+      </c>
+      <c r="B82">
+        <v>0.1939972353703647</v>
+      </c>
+      <c r="C82" t="b">
+        <v>1</v>
+      </c>
+      <c r="D82">
+        <v>0.2977020241362294</v>
+      </c>
+      <c r="E82" t="s">
+        <v>13</v>
+      </c>
+      <c r="F82">
+        <v>0.3411185473202347</v>
+      </c>
+      <c r="G82" t="b">
+        <v>0</v>
+      </c>
+      <c r="H82">
+        <v>0.6129648549176954</v>
+      </c>
+      <c r="I82">
+        <v>0</v>
+      </c>
+      <c r="J82">
+        <v>0</v>
+      </c>
+      <c r="K82">
+        <v>3000</v>
+      </c>
+      <c r="L82">
+        <v>10</v>
+      </c>
+      <c r="M82">
+        <v>0.1176470588235294</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13">
+      <c r="A83">
+        <v>86</v>
+      </c>
+      <c r="B83">
+        <v>0.04254699674622253</v>
+      </c>
+      <c r="C83" t="b">
+        <v>1</v>
+      </c>
+      <c r="D83">
+        <v>0.1203097755065927</v>
+      </c>
+      <c r="E83" t="s">
+        <v>13</v>
+      </c>
+      <c r="F83">
+        <v>0.597514290508959</v>
+      </c>
+      <c r="G83" t="b">
+        <v>0</v>
+      </c>
+      <c r="H83">
+        <v>0.546727638080471</v>
+      </c>
+      <c r="I83">
+        <v>0</v>
+      </c>
+      <c r="J83">
+        <v>0</v>
+      </c>
+      <c r="K83">
+        <v>3000</v>
+      </c>
+      <c r="L83">
+        <v>10</v>
+      </c>
+      <c r="M83">
+        <v>0.1162790697674419</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13">
+      <c r="A84">
+        <v>87</v>
+      </c>
+      <c r="B84">
+        <v>0.3720037738178468</v>
+      </c>
+      <c r="C84" t="b">
+        <v>1</v>
+      </c>
+      <c r="D84">
+        <v>0.718278374680727</v>
+      </c>
+      <c r="E84" t="s">
+        <v>13</v>
+      </c>
+      <c r="F84">
+        <v>0.8289945247477269</v>
+      </c>
+      <c r="G84" t="b">
+        <v>0</v>
+      </c>
+      <c r="H84">
+        <v>0.8765108175639132</v>
+      </c>
+      <c r="I84">
+        <v>0</v>
+      </c>
+      <c r="J84">
+        <v>0</v>
+      </c>
+      <c r="K84">
+        <v>3000</v>
+      </c>
+      <c r="L84">
+        <v>10</v>
+      </c>
+      <c r="M84">
+        <v>0.1149425287356322</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13">
+      <c r="A85">
+        <v>88</v>
+      </c>
+      <c r="B85">
+        <v>0.8545743816844371</v>
+      </c>
+      <c r="C85" t="b">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>0.4944923897971308</v>
+      </c>
+      <c r="F85">
+        <v>0.9765103509595314</v>
+      </c>
+      <c r="H85">
+        <v>0.9167373278838388</v>
+      </c>
+      <c r="I85">
+        <v>0</v>
+      </c>
+      <c r="J85">
+        <v>0</v>
+      </c>
+      <c r="K85">
+        <v>3000</v>
+      </c>
+      <c r="L85">
+        <v>10</v>
+      </c>
+      <c r="M85">
+        <v>0.1136363636363636</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13">
+      <c r="A86">
+        <v>89</v>
+      </c>
+      <c r="B86">
+        <v>0.4885392888618113</v>
+      </c>
+      <c r="C86" t="b">
+        <v>1</v>
+      </c>
+      <c r="D86">
+        <v>0.2185904995054534</v>
+      </c>
+      <c r="E86" t="s">
+        <v>13</v>
+      </c>
+      <c r="F86">
+        <v>0.6143612576412</v>
+      </c>
+      <c r="G86" t="b">
+        <v>0</v>
+      </c>
+      <c r="H86">
+        <v>0.9245327570678554</v>
+      </c>
+      <c r="I86">
+        <v>0</v>
+      </c>
+      <c r="J86">
+        <v>0</v>
+      </c>
+      <c r="K86">
+        <v>3000</v>
+      </c>
+      <c r="L86">
+        <v>10</v>
+      </c>
+      <c r="M86">
+        <v>0.1123595505617977</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13">
+      <c r="A87">
+        <v>90</v>
+      </c>
+      <c r="B87">
+        <v>0.8018832190079382</v>
+      </c>
+      <c r="C87" t="b">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>0.7489149048768589</v>
+      </c>
+      <c r="F87">
+        <v>0.8255770547578429</v>
+      </c>
+      <c r="H87">
+        <v>0.6450235550014718</v>
+      </c>
+      <c r="I87">
+        <v>0</v>
+      </c>
+      <c r="J87">
+        <v>0</v>
+      </c>
+      <c r="K87">
+        <v>3000</v>
+      </c>
+      <c r="L87">
+        <v>10</v>
+      </c>
+      <c r="M87">
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13">
+      <c r="A88">
+        <v>91</v>
+      </c>
+      <c r="B88">
+        <v>0.3879385962299686</v>
+      </c>
+      <c r="C88" t="b">
+        <v>1</v>
+      </c>
+      <c r="D88">
+        <v>0.2978661227063318</v>
+      </c>
+      <c r="E88" t="s">
+        <v>13</v>
+      </c>
+      <c r="F88">
+        <v>0.7085313863796281</v>
+      </c>
+      <c r="G88" t="b">
+        <v>0</v>
+      </c>
+      <c r="H88">
+        <v>0.3271434756096916</v>
+      </c>
+      <c r="I88">
+        <v>0</v>
+      </c>
+      <c r="J88">
+        <v>0</v>
+      </c>
+      <c r="K88">
+        <v>3000</v>
+      </c>
+      <c r="L88">
+        <v>10</v>
+      </c>
+      <c r="M88">
+        <v>0.1098901098901099</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13">
+      <c r="A89">
+        <v>92</v>
+      </c>
+      <c r="B89">
+        <v>0.6603878555195062</v>
+      </c>
+      <c r="C89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D89">
+        <v>0.6575662766754612</v>
+      </c>
+      <c r="E89" t="s">
+        <v>13</v>
+      </c>
+      <c r="F89">
+        <v>0.3987532037178331</v>
+      </c>
+      <c r="G89" t="b">
+        <v>0</v>
+      </c>
+      <c r="H89">
+        <v>0.8306796760919832</v>
+      </c>
+      <c r="I89">
+        <v>0</v>
+      </c>
+      <c r="J89">
+        <v>0</v>
+      </c>
+      <c r="K89">
+        <v>3000</v>
+      </c>
+      <c r="L89">
+        <v>10</v>
+      </c>
+      <c r="M89">
+        <v>0.108695652173913</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13">
+      <c r="A90">
+        <v>93</v>
+      </c>
+      <c r="B90">
+        <v>0.904800125205876</v>
+      </c>
+      <c r="C90" t="b">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>0.3971334532327491</v>
+      </c>
+      <c r="F90">
+        <v>0.1818470119059724</v>
+      </c>
+      <c r="H90">
+        <v>0.5443239475187139</v>
+      </c>
+      <c r="I90">
+        <v>0</v>
+      </c>
+      <c r="J90">
+        <v>0</v>
+      </c>
+      <c r="K90">
+        <v>3000</v>
+      </c>
+      <c r="L90">
+        <v>10</v>
+      </c>
+      <c r="M90">
+        <v>0.1075268817204301</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13">
+      <c r="A91">
+        <v>94</v>
+      </c>
+      <c r="B91">
+        <v>0.6294433405777714</v>
+      </c>
+      <c r="C91" t="b">
+        <v>1</v>
+      </c>
+      <c r="D91">
+        <v>0.9615291741094369</v>
+      </c>
+      <c r="E91" t="s">
+        <v>14</v>
+      </c>
+      <c r="F91">
+        <v>0.7494663047078605</v>
+      </c>
+      <c r="G91" t="b">
+        <v>0</v>
+      </c>
+      <c r="H91">
+        <v>0.6714550007534907</v>
+      </c>
+      <c r="I91">
+        <v>0</v>
+      </c>
+      <c r="J91">
+        <v>0</v>
+      </c>
+      <c r="K91">
+        <v>3000</v>
+      </c>
+      <c r="L91">
+        <v>10</v>
+      </c>
+      <c r="M91">
+        <v>0.1063829787234043</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13">
+      <c r="A92">
+        <v>95</v>
+      </c>
+      <c r="B92">
+        <v>0.1794512377954975</v>
+      </c>
+      <c r="C92" t="b">
+        <v>1</v>
+      </c>
+      <c r="D92">
+        <v>0.4320402527998733</v>
+      </c>
+      <c r="E92" t="s">
+        <v>13</v>
+      </c>
+      <c r="F92">
+        <v>0.0732944031081314</v>
+      </c>
+      <c r="G92" t="b">
+        <v>1</v>
+      </c>
+      <c r="H92">
+        <v>0.3556010716090261</v>
+      </c>
+      <c r="I92">
+        <v>1</v>
+      </c>
+      <c r="J92">
+        <v>200</v>
+      </c>
+      <c r="K92">
+        <v>3200</v>
+      </c>
+      <c r="L92">
+        <v>11</v>
+      </c>
+      <c r="M92">
+        <v>0.1157894736842105</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13">
+      <c r="A93">
+        <v>96</v>
+      </c>
+      <c r="B93">
+        <v>0.8205773312596649</v>
+      </c>
+      <c r="C93" t="b">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>0.8267156820912499</v>
+      </c>
+      <c r="F93">
+        <v>0.1879756110570037</v>
+      </c>
+      <c r="H93">
+        <v>0.4256441290356739</v>
+      </c>
+      <c r="I93">
+        <v>0</v>
+      </c>
+      <c r="J93">
+        <v>0</v>
+      </c>
+      <c r="K93">
+        <v>3200</v>
+      </c>
+      <c r="L93">
+        <v>11</v>
+      </c>
+      <c r="M93">
+        <v>0.1145833333333333</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13">
+      <c r="A94">
+        <v>97</v>
+      </c>
+      <c r="B94">
+        <v>0.8296117716858282</v>
+      </c>
+      <c r="C94" t="b">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>0.1391205111169057</v>
+      </c>
+      <c r="F94">
+        <v>0.4846879634199913</v>
+      </c>
+      <c r="H94">
+        <v>0.6149924583355354</v>
+      </c>
+      <c r="I94">
+        <v>0</v>
+      </c>
+      <c r="J94">
+        <v>0</v>
+      </c>
+      <c r="K94">
+        <v>3200</v>
+      </c>
+      <c r="L94">
+        <v>11</v>
+      </c>
+      <c r="M94">
+        <v>0.1134020618556701</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13">
+      <c r="A95">
+        <v>98</v>
+      </c>
+      <c r="B95">
+        <v>0.2541347820247667</v>
+      </c>
+      <c r="C95" t="b">
+        <v>1</v>
+      </c>
+      <c r="D95">
+        <v>0.8989563528375309</v>
+      </c>
+      <c r="E95" t="s">
+        <v>14</v>
+      </c>
+      <c r="F95">
+        <v>0.1510260808255535</v>
+      </c>
+      <c r="G95" t="b">
+        <v>1</v>
+      </c>
+      <c r="H95">
+        <v>0.7786189763976838</v>
+      </c>
+      <c r="I95">
+        <v>3</v>
+      </c>
+      <c r="J95">
+        <v>600</v>
+      </c>
+      <c r="K95">
+        <v>3800</v>
+      </c>
+      <c r="L95">
+        <v>12</v>
+      </c>
+      <c r="M95">
+        <v>0.1224489795918367</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13">
+      <c r="A96">
+        <v>99</v>
+      </c>
+      <c r="B96">
+        <v>0.5319550784235477</v>
+      </c>
+      <c r="C96" t="b">
+        <v>1</v>
+      </c>
+      <c r="D96">
+        <v>0.4343140358322953</v>
+      </c>
+      <c r="E96" t="s">
+        <v>13</v>
+      </c>
+      <c r="F96">
+        <v>0.3754293008810856</v>
+      </c>
+      <c r="G96" t="b">
+        <v>0</v>
+      </c>
+      <c r="H96">
+        <v>0.3691366221849866</v>
+      </c>
+      <c r="I96">
+        <v>0</v>
+      </c>
+      <c r="J96">
+        <v>0</v>
+      </c>
+      <c r="K96">
+        <v>3800</v>
+      </c>
+      <c r="L96">
+        <v>12</v>
+      </c>
+      <c r="M96">
+        <v>0.1212121212121212</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13">
+      <c r="A97">
+        <v>100</v>
+      </c>
+      <c r="B97">
+        <v>0.4926466058274818</v>
+      </c>
+      <c r="C97" t="b">
+        <v>1</v>
+      </c>
+      <c r="D97">
+        <v>0.9625271307535179</v>
+      </c>
+      <c r="E97" t="s">
+        <v>14</v>
+      </c>
+      <c r="F97">
+        <v>0.2680414005940707</v>
+      </c>
+      <c r="G97" t="b">
+        <v>0</v>
+      </c>
+      <c r="H97">
+        <v>0.1592081544594558</v>
+      </c>
+      <c r="I97">
+        <v>0</v>
+      </c>
+      <c r="J97">
+        <v>0</v>
+      </c>
+      <c r="K97">
+        <v>3800</v>
+      </c>
+      <c r="L97">
+        <v>12</v>
+      </c>
+      <c r="M97">
+        <v>0.12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corregido un error en la validacion de distribuciones
</commit_message>
<xml_diff>
--- a/Tp3/Tabla de simulacion.xlsx
+++ b/Tp3/Tabla de simulacion.xlsx
@@ -442,7 +442,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -537,13 +537,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.9758</v>
+        <v>0.9540999999999999</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0.6889</v>
+        <v>0.0102</v>
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
@@ -551,7 +551,7 @@
         </is>
       </c>
       <c r="F2" s="2" t="n">
-        <v>0.4645</v>
+        <v>0.8473000000000001</v>
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
@@ -559,7 +559,7 @@
         </is>
       </c>
       <c r="H2" s="2" t="n">
-        <v>0.9338</v>
+        <v>0.5372</v>
       </c>
       <c r="I2" s="2" t="n">
         <v>0</v>
@@ -575,6 +575,395 @@
       </c>
       <c r="M2" s="2" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>0.6614</v>
+      </c>
+      <c r="C3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>0.291</v>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>0.274</v>
+      </c>
+      <c r="G3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>0.0648</v>
+      </c>
+      <c r="C4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>0.7704</v>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>0.0089</v>
+      </c>
+      <c r="G4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>0.8394</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>400</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>400</v>
+      </c>
+      <c r="L4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" s="2" t="n">
+        <v>0.3333</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>0.4305</v>
+      </c>
+      <c r="C5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>0.2918</v>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>0.2583</v>
+      </c>
+      <c r="G5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>0.7566000000000001</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>400</v>
+      </c>
+      <c r="L5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" s="2" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>0.0823</v>
+      </c>
+      <c r="C6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>0.0843</v>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>0.4084</v>
+      </c>
+      <c r="G6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>0.5346</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>400</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" s="2" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>0.3297</v>
+      </c>
+      <c r="C7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>0.3064</v>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>0.6657999999999999</v>
+      </c>
+      <c r="G7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>0.5375</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>400</v>
+      </c>
+      <c r="L7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" s="2" t="n">
+        <v>0.1667</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>0.4241</v>
+      </c>
+      <c r="C8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>0.9013</v>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>0.3023</v>
+      </c>
+      <c r="G8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>0.7023</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>400</v>
+      </c>
+      <c r="L8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" s="2" t="n">
+        <v>0.1429</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>0.447</v>
+      </c>
+      <c r="C9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>0.0415</v>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>0.3402</v>
+      </c>
+      <c r="G9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>0.9486</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>400</v>
+      </c>
+      <c r="L9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M9" s="2" t="n">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>0.3516</v>
+      </c>
+      <c r="C10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>0.8421</v>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>0.6471</v>
+      </c>
+      <c r="G10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>0.008500000000000001</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>400</v>
+      </c>
+      <c r="L10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M10" s="2" t="n">
+        <v>0.1111</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>0.7778</v>
+      </c>
+      <c r="C11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>0.2979</v>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>0.279</v>
+      </c>
+      <c r="G11" s="2" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>0.6501</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2" t="n">
+        <v>400</v>
+      </c>
+      <c r="L11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M11" s="2" t="n">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -683,27 +1072,29 @@
         <v>100</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.1025</v>
+        <v>0.7398</v>
       </c>
       <c r="C2" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0.4434</v>
+        <v>0.7712</v>
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>--</t>
         </is>
       </c>
       <c r="F2" s="2" t="n">
-        <v>0.522</v>
-      </c>
-      <c r="G2" s="2" t="b">
-        <v>0</v>
+        <v>0.1989</v>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
       </c>
       <c r="H2" s="2" t="n">
-        <v>0.5137</v>
+        <v>0.9676</v>
       </c>
       <c r="I2" s="2" t="n">
         <v>0</v>
@@ -715,10 +1106,10 @@
         <v>3200</v>
       </c>
       <c r="L2" s="2" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>0.11</v>
+        <v>0.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>